<commit_message>
update getStrData pour prendre en compte la PK et autre modif
quand pas de name prendre index data=1
update CRUD ACT FOU MOY et ZZ TEMPLATE
supression du name dans les NAV.goToURL... et
KW.verifyElementText(NAV.myGlobalJDD,'a_Resultat_ID'
update getData pour prendre en compte getDataLineNum
update GLOBAL nbrecordsGRID_1 et REC
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.GLOBAL.xlsx
+++ b/TNR_JDD/JDD.GLOBAL.xlsx
@@ -169,13 +169,13 @@
     <t>//input[@name='SEARCH_${idname}']</t>
   </si>
   <si>
-    <t>nbrecordsGRID</t>
+    <t>//div[@id='v-dbtdhtmlxGRID']/table/tbody//td[4][text()='${idnameval}']</t>
   </si>
   <si>
-    <t>//strong[@id='dbtdhtmlx_nbrecordsGRID']</t>
+    <t>//strong[@id='dbtdhtmlx_nbrecordsGRID'][text()='1']</t>
   </si>
   <si>
-    <t>//div[@id='v-dbtdhtmlxGRID']/table/tbody//td[4][text()='${idnameval}']</t>
+    <t>nbrecordsGRID_1</t>
   </si>
 </sst>
 </file>
@@ -5699,7 +5699,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -5835,7 +5835,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>47</v>
@@ -5849,7 +5849,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suite à lecture du fichier Result commenté
Prise en compte des nouveaux JDD remodifié suite aux maj précédentes
Ajout des rubriques manquantes MAT et EQU
Ajout des écrans modifi MAT et EQU
Ajouter un STEP pour l'ouverture des fentres de saisie voir Ajouter
Emplacement
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.GLOBAL.xlsx
+++ b/TNR_JDD/JDD.GLOBAL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -231,18 +231,6 @@
   </si>
   <si>
     <t>//div[@class='dhxwin_inactive']</t>
-  </si>
-  <si>
-    <t>checkboxImgChecked</t>
-  </si>
-  <si>
-    <t>${imgXpath}[ends-with(@src,'133.gif')]</t>
-  </si>
-  <si>
-    <t>checkboxImgUnchecked</t>
-  </si>
-  <si>
-    <t>${imgXpath}[ends-with(@src,'134.gif')]</t>
   </si>
 </sst>
 </file>
@@ -31149,28 +31137,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>68</v>
-      </c>
-    </row>
+    <row r="20" ht="12.75" customHeight="1"/>
+    <row r="21" ht="12.75" customHeight="1"/>
     <row r="22" ht="12.75" customHeight="1"/>
     <row r="23" ht="12.75" customHeight="1"/>
     <row r="24" ht="12.75" customHeight="1"/>

</xml_diff>